<commit_message>
POSt Of reconciliation Steps
</commit_message>
<xml_diff>
--- a/RobocorpTestRobots/OBNK-Sheet.xlsx
+++ b/RobocorpTestRobots/OBNK-Sheet.xlsx
@@ -15,9 +15,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="\w\r\a\p_te\x\t\=\T\r\ue"/>
-  </numFmts>
+  <numFmts count="0"/>
   <fonts count="5">
     <font>
       <name val="Calibri"/>
@@ -73,14 +71,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -97,9 +92,6 @@
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
@@ -488,7 +480,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G8"/>
+  <dimension ref="A1:G9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D8" sqref="D8"/>
@@ -505,30 +497,30 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="12" t="inlineStr">
+      <c r="A1" s="10" t="inlineStr">
         <is>
           <t>Bank statement:</t>
         </is>
       </c>
-      <c r="B1" s="10" t="n">
+      <c r="B1" s="8" t="n">
         <v>161012</v>
       </c>
-      <c r="C1" s="10" t="n"/>
+      <c r="C1" s="8" t="n"/>
       <c r="E1" s="1" t="n"/>
-      <c r="F1" s="11" t="n"/>
-      <c r="G1" s="11" t="n"/>
+      <c r="F1" s="9" t="n"/>
+      <c r="G1" s="9" t="n"/>
     </row>
     <row r="2">
-      <c r="A2" s="12" t="n"/>
+      <c r="A2" s="10" t="n"/>
       <c r="B2" s="1" t="inlineStr">
         <is>
           <t>From Date:</t>
         </is>
       </c>
-      <c r="C2" s="4" t="n">
-        <v>45071</v>
-      </c>
-      <c r="G2" s="11" t="n"/>
+      <c r="C2" s="3" t="n">
+        <v>45075</v>
+      </c>
+      <c r="G2" s="9" t="n"/>
     </row>
     <row r="3">
       <c r="A3" s="1" t="n"/>
@@ -537,106 +529,137 @@
           <t>To Date:</t>
         </is>
       </c>
-      <c r="C3" s="4" t="n">
-        <v>45072</v>
+      <c r="C3" s="3" t="n">
+        <v>45077</v>
       </c>
       <c r="E3" s="1" t="n"/>
-      <c r="F3" s="11" t="n"/>
-      <c r="G3" s="11" t="n"/>
+      <c r="F3" s="9" t="n"/>
+      <c r="G3" s="9" t="n"/>
     </row>
     <row r="4">
       <c r="A4" s="1" t="n"/>
-      <c r="B4" s="10" t="n"/>
-      <c r="C4" s="10" t="n"/>
+      <c r="B4" s="8" t="n"/>
+      <c r="C4" s="8" t="n"/>
       <c r="E4" s="1" t="n"/>
-      <c r="F4" s="11" t="n"/>
-      <c r="G4" s="11" t="n"/>
+      <c r="F4" s="9" t="n"/>
+      <c r="G4" s="9" t="n"/>
     </row>
     <row r="5">
-      <c r="A5" s="1" t="inlineStr">
+      <c r="A5" s="10" t="inlineStr">
         <is>
           <t>Transaction ID</t>
         </is>
       </c>
-      <c r="B5" s="1" t="inlineStr">
+      <c r="B5" s="10" t="inlineStr">
         <is>
           <t>Transaction date</t>
         </is>
       </c>
-      <c r="C5" s="1" t="inlineStr">
+      <c r="C5" s="10" t="inlineStr">
         <is>
           <t>Reference No.</t>
         </is>
       </c>
-      <c r="D5" s="2" t="inlineStr">
+      <c r="D5" s="5" t="inlineStr">
         <is>
           <t>Details</t>
         </is>
       </c>
-      <c r="E5" s="1" t="inlineStr">
+      <c r="E5" s="10" t="inlineStr">
         <is>
           <t xml:space="preserve">Debit </t>
         </is>
       </c>
-      <c r="F5" s="1" t="inlineStr">
+      <c r="F5" s="10" t="inlineStr">
         <is>
           <t>Credit</t>
         </is>
       </c>
-      <c r="G5" s="6" t="inlineStr">
+      <c r="G5" s="5" t="inlineStr">
         <is>
           <t>STATUS</t>
         </is>
       </c>
     </row>
     <row r="6" ht="15.75" customHeight="1">
-      <c r="A6" s="3" t="n">
-        <v>25015</v>
-      </c>
-      <c r="B6" s="4" t="n">
-        <v>45071</v>
-      </c>
-      <c r="C6" s="3" t="n">
-        <v>2033</v>
-      </c>
-      <c r="D6" s="5" t="inlineStr">
+      <c r="A6" s="2" t="n">
+        <v>25545</v>
+      </c>
+      <c r="B6" s="3" t="n">
+        <v>45075</v>
+      </c>
+      <c r="C6" s="2" t="n">
+        <v>2034</v>
+      </c>
+      <c r="D6" s="4" t="inlineStr">
         <is>
           <t>Incoming Payment</t>
         </is>
       </c>
-      <c r="E6" s="5" t="n"/>
-      <c r="F6" s="5" t="n">
-        <v>2000</v>
-      </c>
-      <c r="G6" s="8" t="n"/>
+      <c r="E6" s="4" t="n"/>
+      <c r="F6" s="4" t="n">
+        <v>240</v>
+      </c>
+      <c r="G6" s="7" t="n"/>
     </row>
     <row r="7">
-      <c r="A7" s="3" t="n">
-        <v>25016</v>
-      </c>
-      <c r="B7" s="4" t="n">
-        <v>45071</v>
-      </c>
-      <c r="C7" s="3" t="n"/>
-      <c r="D7" s="7" t="inlineStr">
+      <c r="A7" s="2" t="n">
+        <v>25546</v>
+      </c>
+      <c r="B7" s="3" t="n">
+        <v>45075</v>
+      </c>
+      <c r="C7" s="2" t="n"/>
+      <c r="D7" s="6" t="inlineStr">
         <is>
           <t>Bank Charge</t>
         </is>
       </c>
-      <c r="E7" s="5" t="n">
-        <v>50</v>
-      </c>
-      <c r="F7" s="5" t="n"/>
-      <c r="G7" s="8" t="n"/>
+      <c r="E7" s="4" t="n">
+        <v>20</v>
+      </c>
+      <c r="F7" s="4" t="n"/>
+      <c r="G7" s="7" t="n"/>
     </row>
     <row r="8">
-      <c r="A8" s="3" t="n"/>
-      <c r="B8" s="4" t="n"/>
-      <c r="C8" s="4" t="n"/>
-      <c r="D8" s="5" t="n"/>
-      <c r="E8" s="5" t="n"/>
-      <c r="F8" s="5" t="n"/>
-      <c r="G8" s="9" t="n"/>
+      <c r="A8" s="2" t="n">
+        <v>25545</v>
+      </c>
+      <c r="B8" s="3" t="n">
+        <v>45077</v>
+      </c>
+      <c r="C8" s="2" t="n">
+        <v>2034</v>
+      </c>
+      <c r="D8" s="4" t="inlineStr">
+        <is>
+          <t>Incoming Payment</t>
+        </is>
+      </c>
+      <c r="E8" s="4" t="n"/>
+      <c r="F8" s="4" t="n">
+        <v>12000</v>
+      </c>
+      <c r="G8" s="7" t="n"/>
+    </row>
+    <row r="9">
+      <c r="A9" s="2" t="n">
+        <v>25546</v>
+      </c>
+      <c r="B9" s="3" t="n">
+        <v>45077</v>
+      </c>
+      <c r="C9" s="2" t="n"/>
+      <c r="D9" s="6" t="inlineStr">
+        <is>
+          <t>Bank Charge</t>
+        </is>
+      </c>
+      <c r="E9" s="4" t="n">
+        <v>250</v>
+      </c>
+      <c r="F9" s="4" t="n"/>
+      <c r="G9" s="7" t="n"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>